<commit_message>
fix: insert data to excel
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -12,6 +12,83 @@
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>KEUDE BAKONGAN</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[186 44 8]]]</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[186 44 8]] map[TPS2:[209 37 6]]]</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[186 44 8]] map[TPS2:[209 37 6]] map[TPS3:[202 38 7]]]</t>
+  </si>
+  <si>
+    <t>GAMPONG DRIEN</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[144 19 2]]]</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[144 19 2]] map[TPS2:[153 14 4]]]</t>
+  </si>
+  <si>
+    <t>DARUL IKHSAN</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[210 33 4]]]</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[210 33 4]] map[TPS2:[207 31 1]]]</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[210 33 4]] map[TPS2:[207 31 1]] map[TPS3:[200 33 0]]]</t>
+  </si>
+  <si>
+    <t>PADANG BEURAHAN</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[204 39 2]]]</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[204 39 2]] map[TPS2:[203 36 1]]]</t>
+  </si>
+  <si>
+    <t>GAMPONG BARO</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[199 41 2]]]</t>
+  </si>
+  <si>
+    <t>FAJAR HARAPAN</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[197 31 2]]]</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[197 31 2]] map[TPS2:[196 26 1]]]</t>
+  </si>
+  <si>
+    <t>KRUENG BATEE</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[212 16 2]]]</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[212 16 2]] map[TPS2:[225 12 2]]]</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[212 16 2]] map[TPS2:[225 12 2]] map[TPS3:[229 10 1]]]</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[212 16 2]] map[TPS2:[225 12 2]] map[TPS3:[229 10 1]] map[TPS4:[240 17 2]]]</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -328,6 +405,159 @@
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1101012001</v>
+      </c>
+      <c r="C2">
+        <v>873</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>284</v>
+      </c>
+      <c r="F2">
+        <v>296</v>
+      </c>
+      <c r="G2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1101012004</v>
+      </c>
+      <c r="C5">
+        <v>363</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>182</v>
+      </c>
+      <c r="F5">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1101012015</v>
+      </c>
+      <c r="C6">
+        <v>803</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>271</v>
+      </c>
+      <c r="F6">
+        <v>265</v>
+      </c>
+      <c r="G6">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>1101012016</v>
+      </c>
+      <c r="C7">
+        <v>549</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7">
+        <v>278</v>
+      </c>
+      <c r="F7">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>1101012017</v>
+      </c>
+      <c r="C8">
+        <v>260</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>1101022001</v>
+      </c>
+      <c r="C9">
+        <v>517</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9">
+        <v>254</v>
+      </c>
+      <c r="F9">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>1101022002</v>
+      </c>
+      <c r="C10">
+        <v>1102</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10">
+        <v>271</v>
+      </c>
+      <c r="F10">
+        <v>277</v>
+      </c>
+      <c r="G10">
+        <v>266</v>
+      </c>
+      <c r="H10">
+        <v>288</v>
+      </c>
+    </row>
+  </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add concurrency on multitask scraping
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -15,39 +15,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>UJONG MANGKI</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[212 36 1]] map[TPS2:[235 26 7]]]</t>
+  </si>
+  <si>
+    <t>GAMPONG DRIEN</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[144 19 2]] map[TPS2:[153 14 4]]]</t>
+  </si>
+  <si>
+    <t>DARUL IKHSAN</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[210 33 4]] map[TPS2:[207 31 1]] map[TPS3:[200 33 0]]]</t>
+  </si>
+  <si>
+    <t>PADANG BEURAHAN</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[204 39 2]] map[TPS2:[203 36 1]]]</t>
+  </si>
+  <si>
+    <t>GAMPONG BARO</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[199 41 2]]]</t>
+  </si>
+  <si>
+    <t>FAJAR HARAPAN</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[197 31 2]] map[TPS2:[196 26 1]]]</t>
+  </si>
+  <si>
+    <t>KRUENG BATEE</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[212 16 2]] map[TPS2:[225 12 2]] map[TPS3:[229 10 1]] map[TPS4:[240 17 2]]]</t>
+  </si>
+  <si>
+    <t>PASI KUALA ASAHAN</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[235 15 2]] map[TPS2:[197 17 3]]]</t>
+  </si>
+  <si>
+    <t>KEUDE BAKONGAN</t>
+  </si>
+  <si>
+    <t>[map[TPS1:[186 44 8]] map[TPS2:[209 37 6]] map[TPS3:[202 38 7]]]</t>
+  </si>
   <si>
     <t>UJONG PADANG</t>
   </si>
   <si>
     <t>[map[TPS1:[176 27 3]] map[TPS2:[185 29 4]]]</t>
-  </si>
-  <si>
-    <t>GAMPONG DRIEN</t>
-  </si>
-  <si>
-    <t>[map[TPS2:[153 14 4]]]</t>
-  </si>
-  <si>
-    <t>DARUL IKHSAN</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>PADANG BEURAHAN</t>
-  </si>
-  <si>
-    <t>[map[TPS2:[203 36 1]]]</t>
-  </si>
-  <si>
-    <t>GAMPONG BARO</t>
-  </si>
-  <si>
-    <t>FAJAR HARAPAN</t>
-  </si>
-  <si>
-    <t>KRUENG BATEE</t>
   </si>
 </sst>
 </file>
@@ -368,11 +395,52 @@
   </sheetViews>
   <sheetData>
     <row r="1"/>
-    <row r="2"/>
-    <row r="3"/>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1101012001</v>
+      </c>
+      <c r="C2">
+        <v>873</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>284</v>
+      </c>
+      <c r="F2">
+        <v>296</v>
+      </c>
+      <c r="G2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1101012002</v>
+      </c>
+      <c r="C3">
+        <v>562</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>268</v>
+      </c>
+      <c r="F3">
+        <v>294</v>
+      </c>
+    </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>1101012003</v>
@@ -381,7 +449,7 @@
         <v>476</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>230</v>
@@ -398,13 +466,16 @@
         <v>1101012004</v>
       </c>
       <c r="C5">
-        <v>181</v>
+        <v>363</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>182</v>
+      </c>
+      <c r="F5">
+        <v>181</v>
       </c>
     </row>
     <row r="6">
@@ -415,10 +486,19 @@
         <v>1101012015</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>803</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
+      </c>
+      <c r="E6">
+        <v>271</v>
+      </c>
+      <c r="F6">
+        <v>265</v>
+      </c>
+      <c r="G6">
+        <v>267</v>
       </c>
     </row>
     <row r="7">
@@ -429,13 +509,16 @@
         <v>1101012016</v>
       </c>
       <c r="C7">
-        <v>271</v>
+        <v>549</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>278</v>
+      </c>
+      <c r="F7">
+        <v>271</v>
       </c>
     </row>
     <row r="8">
@@ -446,38 +529,79 @@
         <v>1101012017</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>260</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>260</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>1101022001</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>517</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>254</v>
+      </c>
+      <c r="F9">
+        <v>263</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>1101022002</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1102</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>271</v>
+      </c>
+      <c r="F10">
+        <v>277</v>
+      </c>
+      <c r="G10">
+        <v>266</v>
+      </c>
+      <c r="H10">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>1101022003</v>
+      </c>
+      <c r="C11">
+        <v>549</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>282</v>
+      </c>
+      <c r="F11">
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>